<commit_message>
excel, lvl 3 stage clear and reactivate
</commit_message>
<xml_diff>
--- a/TimeTable_GosseBump_Games.xlsx
+++ b/TimeTable_GosseBump_Games.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martí\Desktop\Andro_Dunos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907E28A6-08F2-450E-A927-4F08A073D256}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Full 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Full 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="176">
   <si>
     <r>
       <t xml:space="preserve">
@@ -19,7 +28,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="15.0"/>
+        <sz val="15"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>BEFORE ALPHA</t>
     </r>
@@ -394,9 +404,6 @@
     <t>ALL</t>
   </si>
   <si>
-    <t>J: 2h G: 1h</t>
-  </si>
-  <si>
     <t>-Fix spaceship turbo</t>
   </si>
   <si>
@@ -481,9 +488,6 @@
     <t>-//1/2 enemies (20-27)</t>
   </si>
   <si>
-    <t>G: 4h</t>
-  </si>
-  <si>
     <t>0.9</t>
   </si>
   <si>
@@ -532,48 +536,77 @@
     <t>3h 30min</t>
   </si>
   <si>
-    <t>10min (fullscreen)</t>
-  </si>
-  <si>
     <t>26h</t>
   </si>
   <si>
     <t>33h 30min</t>
+  </si>
+  <si>
+    <t>23h</t>
+  </si>
+  <si>
+    <t>7h 50min</t>
+  </si>
+  <si>
+    <t>Jorge/Gerard/Martí</t>
+  </si>
+  <si>
+    <t>G: 4h M: 1h 30 min</t>
+  </si>
+  <si>
+    <t>J: 2h G: 1h  M: 1h</t>
+  </si>
+  <si>
+    <t>36h 20 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="24.0"/>
+      <sz val="24"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -582,7 +615,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -592,85 +625,383 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="K92" sqref="K92"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="39.29"/>
-    <col customWidth="1" min="2" max="2" width="26.29"/>
-    <col customWidth="1" min="6" max="6" width="16.14"/>
-    <col customWidth="1" min="8" max="8" width="16.14"/>
-    <col customWidth="1" min="9" max="9" width="15.86"/>
-    <col customWidth="1" min="10" max="10" width="19.14"/>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -696,7 +1027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -710,7 +1041,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="5">
-        <v>43204.0</v>
+        <v>43204</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>12</v>
@@ -722,7 +1053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -736,7 +1067,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="5">
-        <v>43210.0</v>
+        <v>43210</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>18</v>
@@ -748,7 +1079,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -762,7 +1093,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="5">
-        <v>43211.0</v>
+        <v>43211</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>24</v>
@@ -774,7 +1105,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -800,7 +1131,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -817,7 +1148,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>35</v>
       </c>
@@ -834,7 +1165,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -851,7 +1182,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
@@ -868,7 +1199,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
@@ -885,7 +1216,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -902,7 +1233,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
@@ -919,7 +1250,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>49</v>
       </c>
@@ -936,7 +1267,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -953,7 +1284,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
@@ -970,7 +1301,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>55</v>
       </c>
@@ -987,7 +1318,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>56</v>
       </c>
@@ -1004,7 +1335,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>58</v>
       </c>
@@ -1021,7 +1352,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>60</v>
       </c>
@@ -1038,7 +1369,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>61</v>
       </c>
@@ -1055,7 +1386,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>63</v>
       </c>
@@ -1072,7 +1403,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>65</v>
       </c>
@@ -1089,7 +1420,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>66</v>
       </c>
@@ -1106,7 +1437,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>67</v>
       </c>
@@ -1123,7 +1454,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>68</v>
       </c>
@@ -1140,7 +1471,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>69</v>
       </c>
@@ -1157,7 +1488,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>70</v>
       </c>
@@ -1174,7 +1505,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>72</v>
       </c>
@@ -1191,7 +1522,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>74</v>
       </c>
@@ -1208,7 +1539,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>75</v>
       </c>
@@ -1225,7 +1556,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>76</v>
       </c>
@@ -1242,7 +1573,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
@@ -1259,14 +1590,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>78</v>
       </c>
@@ -1278,10 +1609,10 @@
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="6">
-        <v>43106.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>43106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>81</v>
       </c>
@@ -1292,7 +1623,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>82</v>
       </c>
@@ -1303,7 +1634,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>83</v>
       </c>
@@ -1320,7 +1651,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>85</v>
       </c>
@@ -1337,7 +1668,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>87</v>
       </c>
@@ -1348,7 +1679,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>88</v>
       </c>
@@ -1359,7 +1690,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>89</v>
       </c>
@@ -1376,7 +1707,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>91</v>
       </c>
@@ -1393,7 +1724,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>93</v>
       </c>
@@ -1404,7 +1735,7 @@
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>94</v>
       </c>
@@ -1421,7 +1752,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>96</v>
       </c>
@@ -1432,7 +1763,7 @@
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>97</v>
       </c>
@@ -1449,7 +1780,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>100</v>
       </c>
@@ -1460,7 +1791,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>102</v>
       </c>
@@ -1477,7 +1808,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>104</v>
       </c>
@@ -1488,7 +1819,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>105</v>
       </c>
@@ -1500,10 +1831,10 @@
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="6">
-        <v>43106.0</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>43106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>106</v>
       </c>
@@ -1515,10 +1846,10 @@
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="6">
-        <v>43106.0</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>43106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
@@ -1535,7 +1866,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>109</v>
       </c>
@@ -1552,12 +1883,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>113</v>
       </c>
@@ -1580,13 +1911,18 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="10" t="s">
+    <row r="58" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="13" t="s">
         <v>119</v>
       </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
       <c r="I58" s="1" t="s">
         <v>120</v>
       </c>
@@ -1597,10 +1933,16 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59">
-      <c r="B59" s="1" t="s">
+    <row r="59" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="13" t="s">
         <v>122</v>
       </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
       <c r="I59" s="1" t="s">
         <v>123</v>
       </c>
@@ -1608,13 +1950,19 @@
         <v>39</v>
       </c>
       <c r="K59" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="13" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="60">
-      <c r="B60" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
       <c r="I60" s="1" t="s">
         <v>18</v>
       </c>
@@ -1625,52 +1973,76 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61">
-      <c r="B61" s="1" t="s">
+    <row r="61" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="I61" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K61" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="13" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="62">
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="I62" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>80</v>
       </c>
       <c r="K62" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="13" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="63">
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="I63" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K63" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="13" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="64">
-      <c r="B64" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
       <c r="I64" s="1" t="s">
         <v>9</v>
       </c>
@@ -1681,10 +2053,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65">
-      <c r="B65" s="1" t="s">
-        <v>136</v>
-      </c>
+    <row r="65" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
       <c r="I65" s="1" t="s">
         <v>12</v>
       </c>
@@ -1692,13 +2070,19 @@
         <v>47</v>
       </c>
       <c r="K65" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="13" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="66">
-      <c r="B66" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
       <c r="I66" s="1" t="s">
         <v>18</v>
       </c>
@@ -1706,16 +2090,21 @@
         <v>59</v>
       </c>
       <c r="K66" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="10" t="s">
+      <c r="B68" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>141</v>
-      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
       <c r="I68" s="1" t="s">
         <v>24</v>
       </c>
@@ -1723,13 +2112,19 @@
         <v>11</v>
       </c>
       <c r="K68" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A69" s="14"/>
+      <c r="B69" s="13" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="69">
-      <c r="B69" s="1" t="s">
-        <v>143</v>
-      </c>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
       <c r="I69" s="1" t="s">
         <v>9</v>
       </c>
@@ -1740,24 +2135,36 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70">
-      <c r="B70" s="1" t="s">
-        <v>144</v>
-      </c>
+    <row r="70" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A70" s="14"/>
+      <c r="B70" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
       <c r="I70" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>80</v>
       </c>
       <c r="K70" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A71" s="14"/>
+      <c r="B71" s="13" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="71">
-      <c r="B71" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
       <c r="I71" s="1" t="s">
         <v>9</v>
       </c>
@@ -1768,16 +2175,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.5">
       <c r="A72" s="10"/>
     </row>
-    <row r="73">
-      <c r="A73" s="10" t="s">
+    <row r="73" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
       <c r="I73" s="1" t="s">
         <v>24</v>
       </c>
@@ -1788,62 +2200,97 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74">
-      <c r="B74" s="1" t="s">
+    <row r="74" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A74" s="14"/>
+      <c r="B74" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="I74" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I74" s="1" t="s">
+    </row>
+    <row r="75" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A75" s="14"/>
+      <c r="B75" s="15" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="75">
-      <c r="B75" s="11" t="s">
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="I75" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A76" s="14"/>
+      <c r="B76" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="I75" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" s="11" t="s">
-        <v>152</v>
-      </c>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
       <c r="I76" s="1" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K76" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="13" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="10" t="s">
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="I78" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K78" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+    </row>
+    <row r="80" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A80" s="14"/>
+      <c r="B80" s="15" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="79">
-      <c r="B79" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="B80" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
       <c r="I80" s="1" t="s">
         <v>24</v>
       </c>
@@ -1851,29 +2298,52 @@
         <v>17</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="B81" s="11" t="s">
-        <v>161</v>
-      </c>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A81" s="14"/>
+      <c r="B81" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
       <c r="I81" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="10" t="s">
+      <c r="J81" t="s">
+        <v>39</v>
+      </c>
+      <c r="K81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A83" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+    </row>
+    <row r="84" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A84" s="14"/>
+      <c r="B84" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="B84" s="1" t="s">
-        <v>164</v>
-      </c>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
       <c r="I84" s="1" t="s">
         <v>9</v>
       </c>
@@ -1884,12 +2354,18 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85">
-      <c r="B85" s="1" t="s">
-        <v>165</v>
-      </c>
+    <row r="85" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A85" s="14"/>
+      <c r="B85" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
       <c r="I85" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>59</v>
@@ -1898,22 +2374,30 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86">
-      <c r="B86" s="11" t="s">
-        <v>167</v>
-      </c>
+    <row r="86" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A86" s="14"/>
+      <c r="B86" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
       <c r="I86" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="89">
-      <c r="B89" s="8"/>
+    <row r="89" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B89" s="17"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
       <c r="I89" s="2" t="s">
         <v>6</v>
       </c>
@@ -1924,58 +2408,53 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="I90" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J90" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K90" s="4"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="I91" s="4" t="s">
         <v>18</v>
       </c>
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
     </row>
-    <row r="92">
+    <row r="92" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="I92" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J92" s="12" t="s">
+      <c r="J92" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="K92" s="4"/>
-    </row>
-    <row r="93">
+      <c r="K92" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="I93" s="4" t="s">
         <v>9</v>
       </c>
       <c r="J93" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K93" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B85:G85"/>
-    <mergeCell ref="B86:G86"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="B79:G79"/>
-    <mergeCell ref="B78:G78"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B74:G74"/>
-    <mergeCell ref="B75:G75"/>
-    <mergeCell ref="B81:G81"/>
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B84:G84"/>
-    <mergeCell ref="B80:G80"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="A58:A66"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="B71:G71"/>
     <mergeCell ref="B68:G68"/>
     <mergeCell ref="B65:G65"/>
     <mergeCell ref="B66:G66"/>
@@ -1986,14 +2465,21 @@
     <mergeCell ref="B61:G61"/>
     <mergeCell ref="B62:G62"/>
     <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="A58:A66"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B74:G74"/>
+    <mergeCell ref="B75:G75"/>
+    <mergeCell ref="B81:G81"/>
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B84:G84"/>
+    <mergeCell ref="B80:G80"/>
+    <mergeCell ref="B85:G85"/>
+    <mergeCell ref="B86:G86"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="B79:G79"/>
+    <mergeCell ref="B78:G78"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>